<commit_message>
Metodo A* parte 2
</commit_message>
<xml_diff>
--- a/tarea01 - algoritomo A/metodos A.xlsx
+++ b/tarea01 - algoritomo A/metodos A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\saids\Desktop\InteligenciaArtificalClass-Repo\tarea01 - algoritomo A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36076AF2-A701-49AF-9490-5C0EA8B41F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C0D3E8-6454-4B78-A826-837840152992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E48C7606-B267-4B67-A036-034A0E98C5EC}"/>
   </bookViews>
@@ -1244,8 +1244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B60A026-C6D3-4829-9E1E-5AEC7B07DCED}">
   <dimension ref="B2:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1940,9 +1940,7 @@
       <c r="H27" s="30">
         <v>8</v>
       </c>
-      <c r="I27" s="30">
-        <v>1</v>
-      </c>
+      <c r="I27" s="30"/>
       <c r="J27" s="30">
         <v>2</v>
       </c>

</xml_diff>